<commit_message>
* add expenses types to general settings * fetch the rest of expenses fields
</commit_message>
<xml_diff>
--- a/Saudi/Cancel Reservation.xlsx
+++ b/Saudi/Cancel Reservation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Payment Amount</t>
   </si>
@@ -39,6 +39,9 @@
     <t>Discount Amount</t>
   </si>
   <si>
+    <t>Room Tax</t>
+  </si>
+  <si>
     <t>Payment Method</t>
   </si>
   <si>
@@ -51,13 +54,10 @@
     <t>Departure Date</t>
   </si>
   <si>
+    <t>DUP</t>
+  </si>
+  <si>
     <t>CA</t>
-  </si>
-  <si>
-    <t>CL</t>
-  </si>
-  <si>
-    <t>MA</t>
   </si>
 </sst>
 </file>
@@ -553,16 +553,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -892,27 +889,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -943,261 +939,44 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1821.81</v>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>76651</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>76151</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="D2" s="3">
         <v>3</v>
       </c>
       <c r="E2" s="3">
-        <v>479.4</v>
+        <v>630</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1438.2</v>
-      </c>
-      <c r="I2" s="5">
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1890</v>
+      </c>
+      <c r="J2" s="4">
         <v>43547</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="4">
         <v>43550</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3">
-        <v>75651</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>379.62</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="3">
-        <v>759.24</v>
-      </c>
-      <c r="I3" s="5">
-        <v>43548</v>
-      </c>
-      <c r="J3" s="5">
-        <v>43550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3">
-        <v>75401</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>377.4</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="3">
-        <v>377.4</v>
-      </c>
-      <c r="I4" s="5">
-        <v>43547</v>
-      </c>
-      <c r="J4" s="5">
-        <v>43548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
-        <v>75151</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>488.83</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1466.49</v>
-      </c>
-      <c r="I5" s="5">
-        <v>43547</v>
-      </c>
-      <c r="J5" s="5">
-        <v>43550</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3">
-        <v>74902</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>330.62</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3">
-        <v>661.24</v>
-      </c>
-      <c r="I6" s="5">
-        <v>43547</v>
-      </c>
-      <c r="J6" s="5">
-        <v>43549</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0</v>
-      </c>
-      <c r="B7" s="3">
-        <v>74901</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>330.62</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3">
-        <v>661.24</v>
-      </c>
-      <c r="I7" s="5">
-        <v>43547</v>
-      </c>
-      <c r="J7" s="5">
-        <v>43549</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0</v>
-      </c>
-      <c r="B8" s="3">
-        <v>74651</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3">
-        <v>266.39999999999998</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="3">
-        <v>799.2</v>
-      </c>
-      <c r="I8" s="5">
-        <v>43547</v>
-      </c>
-      <c r="J8" s="5">
-        <v>43550</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3">
-        <v>77151</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3">
-        <v>510</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2040</v>
-      </c>
-      <c r="I9" s="5">
-        <v>43547</v>
-      </c>
-      <c r="J9" s="5">
-        <v>43551</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1609.4</v>
-      </c>
-      <c r="B10" s="3">
-        <v>68653</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3">
-        <v>377.4</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1132.2</v>
-      </c>
-      <c r="I10" s="5">
-        <v>43546</v>
-      </c>
-      <c r="J10" s="5">
-        <v>43549</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>